<commit_message>
Postdoc cost of living data
</commit_message>
<xml_diff>
--- a/Raw_Data/rent_cities.xlsx
+++ b/Raw_Data/rent_cities.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\SoS_funding\Raw_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA0E80F-7C31-494F-B943-E04F167BD1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EC9E4B-AB23-489D-BEF9-A55E5B8BF40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D3D01D50-B2A4-447A-A774-83900E9EBD2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D3D01D50-B2A4-447A-A774-83900E9EBD2D}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="meta" sheetId="2" r:id="rId2"/>
+    <sheet name="grad" sheetId="1" r:id="rId1"/>
+    <sheet name="pdf" sheetId="3" r:id="rId2"/>
+    <sheet name="CoL" sheetId="4" r:id="rId3"/>
+    <sheet name="meta" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="71">
   <si>
     <t>Province</t>
   </si>
@@ -179,9 +181,6 @@
     <t>PDF amount (CAD)</t>
   </si>
   <si>
-    <t>Average 1 bedroom rent from Zumper as of July 21, 2022</t>
-  </si>
-  <si>
     <t>https://www.zumper.com/rent-research/vancouver-bc</t>
   </si>
   <si>
@@ -207,13 +206,58 @@
   </si>
   <si>
     <t>Full-time Canadian grad student tuition fees 2021 - 2022</t>
+  </si>
+  <si>
+    <t>Average 1 bedroom rent from Zumper as of July 21, 2022 for grad students, 2 bedroom for pdf</t>
+  </si>
+  <si>
+    <t>rent</t>
+  </si>
+  <si>
+    <t>transportation</t>
+  </si>
+  <si>
+    <t>grocery</t>
+  </si>
+  <si>
+    <t>preschool</t>
+  </si>
+  <si>
+    <t>Montreal</t>
+  </si>
+  <si>
+    <t>St. John’s</t>
+  </si>
+  <si>
+    <t>Moncton</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t>https://wowa.ca/cost-of-living-canada</t>
+  </si>
+  <si>
+    <t>utilities</t>
+  </si>
+  <si>
+    <t>family of 3 (2 adults 1 child)</t>
+  </si>
+  <si>
+    <t>monthly_col</t>
+  </si>
+  <si>
+    <t>yearly_expenses</t>
+  </si>
+  <si>
+    <t>Charlottestown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +269,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -251,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -259,12 +311,58 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -576,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9201778-9310-443F-99EA-B46A8D563097}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="A1:J27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,10 +718,10 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1467,11 +1565,1262 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F162D4F-4FC6-474B-BB43-16544EB64190}">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478A2521-12DD-4F3D-9984-98BBCEC7701A}">
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C23" sqref="C23:D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>51.078400000000002</v>
+      </c>
+      <c r="D2">
+        <v>-114.1347</v>
+      </c>
+      <c r="E2">
+        <v>45000</v>
+      </c>
+      <c r="F2">
+        <v>1699</v>
+      </c>
+      <c r="G2">
+        <f>F2*12</f>
+        <v>20388</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>53.523200000000003</v>
+      </c>
+      <c r="D3">
+        <v>-113.52630000000001</v>
+      </c>
+      <c r="E3">
+        <v>45000</v>
+      </c>
+      <c r="F3">
+        <v>1250</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G27" si="0">F3*12</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>49.678600000000003</v>
+      </c>
+      <c r="D4">
+        <v>-112.86</v>
+      </c>
+      <c r="E4">
+        <v>45000</v>
+      </c>
+      <c r="F4">
+        <v>1160</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>13920</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>49.278100000000002</v>
+      </c>
+      <c r="D5">
+        <v>-122.9199</v>
+      </c>
+      <c r="E5">
+        <v>45000</v>
+      </c>
+      <c r="F5">
+        <v>2485</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>29820</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6">
+        <v>49.260599999999997</v>
+      </c>
+      <c r="D6">
+        <v>-123.246</v>
+      </c>
+      <c r="E6">
+        <v>45000</v>
+      </c>
+      <c r="F6">
+        <v>3500</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>48.4634</v>
+      </c>
+      <c r="D7">
+        <v>-123.3117</v>
+      </c>
+      <c r="E7">
+        <v>45000</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2550</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>30600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8">
+        <v>49.807499999999997</v>
+      </c>
+      <c r="D8">
+        <v>-97.136600000000001</v>
+      </c>
+      <c r="E8">
+        <v>45000</v>
+      </c>
+      <c r="F8">
+        <v>1375</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>16500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>45.944800000000001</v>
+      </c>
+      <c r="D9">
+        <v>-66.643000000000001</v>
+      </c>
+      <c r="E9">
+        <v>45000</v>
+      </c>
+      <c r="F9">
+        <v>1300</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>15600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10">
+        <v>47.573799999999999</v>
+      </c>
+      <c r="D10">
+        <v>-52.732900000000001</v>
+      </c>
+      <c r="E10">
+        <v>45000</v>
+      </c>
+      <c r="F10">
+        <v>908</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>10896</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>44.636600000000001</v>
+      </c>
+      <c r="D11">
+        <v>-63.591700000000003</v>
+      </c>
+      <c r="E11">
+        <v>45000</v>
+      </c>
+      <c r="F11">
+        <v>2295</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>27540</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>43.532699999999998</v>
+      </c>
+      <c r="D12">
+        <v>-80.226200000000006</v>
+      </c>
+      <c r="E12">
+        <v>45000</v>
+      </c>
+      <c r="F12">
+        <v>2199</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>26388</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>43.260899999999999</v>
+      </c>
+      <c r="D13">
+        <v>-79.919200000000004</v>
+      </c>
+      <c r="E13">
+        <v>45000</v>
+      </c>
+      <c r="F13">
+        <v>1885</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>22620</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <v>44.225299999999997</v>
+      </c>
+      <c r="D14">
+        <v>-76.495099999999994</v>
+      </c>
+      <c r="E14">
+        <v>45000</v>
+      </c>
+      <c r="F14">
+        <v>1828</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>21936</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <v>43.472299999999997</v>
+      </c>
+      <c r="D15">
+        <v>-80.544899999999998</v>
+      </c>
+      <c r="E15">
+        <v>45000</v>
+      </c>
+      <c r="F15">
+        <v>1995</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>23940</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>43.009599999999999</v>
+      </c>
+      <c r="D16">
+        <v>-81.273700000000005</v>
+      </c>
+      <c r="E16">
+        <v>45000</v>
+      </c>
+      <c r="F16">
+        <v>1770</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>21240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>43.945500000000003</v>
+      </c>
+      <c r="D17">
+        <v>-78.896799999999999</v>
+      </c>
+      <c r="E17">
+        <v>45000</v>
+      </c>
+      <c r="F17">
+        <v>1995</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>23940</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18">
+        <v>45.387599999999999</v>
+      </c>
+      <c r="D18">
+        <v>-75.695999999999998</v>
+      </c>
+      <c r="E18">
+        <v>45000</v>
+      </c>
+      <c r="F18">
+        <v>1859</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>22308</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19">
+        <v>43.117600000000003</v>
+      </c>
+      <c r="D19">
+        <v>-79.247699999999995</v>
+      </c>
+      <c r="E19">
+        <v>45000</v>
+      </c>
+      <c r="F19">
+        <v>1885</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>22620</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20">
+        <v>46.467199999999998</v>
+      </c>
+      <c r="D20">
+        <v>-80.975700000000003</v>
+      </c>
+      <c r="E20">
+        <v>45000</v>
+      </c>
+      <c r="F20">
+        <v>1599</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>19188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>43.657699999999998</v>
+      </c>
+      <c r="D21">
+        <v>-79.378799999999998</v>
+      </c>
+      <c r="E21">
+        <v>45000</v>
+      </c>
+      <c r="F21">
+        <v>2499</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>29988</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>42.304299999999998</v>
+      </c>
+      <c r="D22">
+        <v>-83.066000000000003</v>
+      </c>
+      <c r="E22">
+        <v>45000</v>
+      </c>
+      <c r="F22">
+        <v>1575</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>18900</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>46.256900000000002</v>
+      </c>
+      <c r="D23">
+        <v>-63.1389</v>
+      </c>
+      <c r="E23">
+        <v>45000</v>
+      </c>
+      <c r="F23">
+        <v>1290</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>15480</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24">
+        <v>45.494799999999998</v>
+      </c>
+      <c r="D24">
+        <v>-73.5779</v>
+      </c>
+      <c r="E24">
+        <v>45000</v>
+      </c>
+      <c r="F24">
+        <v>1950</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>23400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>45.504800000000003</v>
+      </c>
+      <c r="D25">
+        <v>-73.613200000000006</v>
+      </c>
+      <c r="E25">
+        <v>45000</v>
+      </c>
+      <c r="F25">
+        <v>1425</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>17100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>50.415500000000002</v>
+      </c>
+      <c r="D26">
+        <v>-104.5878</v>
+      </c>
+      <c r="E26">
+        <v>45000</v>
+      </c>
+      <c r="F26">
+        <v>1135</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>13620</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27">
+        <v>52.133400000000002</v>
+      </c>
+      <c r="D27">
+        <v>-106.6314</v>
+      </c>
+      <c r="E27">
+        <v>45000</v>
+      </c>
+      <c r="F27">
+        <v>1137</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>13644</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BFA5AB1-F7F8-42C3-AF45-032CD661A926}">
+  <dimension ref="A1:J30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="29" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>51.078400000000002</v>
+      </c>
+      <c r="C2">
+        <v>-114.1347</v>
+      </c>
+      <c r="D2">
+        <v>1699</v>
+      </c>
+      <c r="E2" s="8">
+        <f>176+180</f>
+        <v>356</v>
+      </c>
+      <c r="F2" s="8">
+        <v>525</v>
+      </c>
+      <c r="G2" s="8">
+        <v>1296</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1145</v>
+      </c>
+      <c r="I2" s="7">
+        <f>SUM(D2:H2)</f>
+        <v>5021</v>
+      </c>
+      <c r="J2">
+        <f>I2*12</f>
+        <v>60252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>53.523200000000003</v>
+      </c>
+      <c r="C3">
+        <v>-113.52630000000001</v>
+      </c>
+      <c r="D3">
+        <v>1250</v>
+      </c>
+      <c r="E3" s="8">
+        <f>176+180</f>
+        <v>356</v>
+      </c>
+      <c r="F3" s="8">
+        <v>525</v>
+      </c>
+      <c r="G3" s="8">
+        <v>1296</v>
+      </c>
+      <c r="H3" s="8">
+        <v>925</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" ref="I3:I15" si="0">SUM(D3:H3)</f>
+        <v>4352</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J15" si="1">I3*12</f>
+        <v>52224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>44.636600000000001</v>
+      </c>
+      <c r="C4">
+        <v>-63.591700000000003</v>
+      </c>
+      <c r="D4">
+        <v>2295</v>
+      </c>
+      <c r="E4" s="8">
+        <f>167+180</f>
+        <v>347</v>
+      </c>
+      <c r="F4" s="8">
+        <v>523</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1041</v>
+      </c>
+      <c r="H4" s="8">
+        <v>868</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="0"/>
+        <v>5074</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>60888</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>43.009599999999999</v>
+      </c>
+      <c r="C5">
+        <v>-81.273700000000005</v>
+      </c>
+      <c r="D5">
+        <v>1770</v>
+      </c>
+      <c r="E5" s="8">
+        <f>89+168</f>
+        <v>257</v>
+      </c>
+      <c r="F5" s="8">
+        <v>578</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1194</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1075</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="0"/>
+        <v>4874</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>58488</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6">
+        <v>46.087800000000001</v>
+      </c>
+      <c r="C6">
+        <v>-64.778199999999998</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1150</v>
+      </c>
+      <c r="E6" s="8">
+        <f>132+171</f>
+        <v>303</v>
+      </c>
+      <c r="F6" s="8">
+        <v>507</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1086</v>
+      </c>
+      <c r="H6" s="8">
+        <v>716</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="0"/>
+        <v>3762</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>45144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7">
+        <v>45.494799999999998</v>
+      </c>
+      <c r="C7">
+        <v>-73.5779</v>
+      </c>
+      <c r="D7">
+        <v>1950</v>
+      </c>
+      <c r="E7" s="8">
+        <f>73+160</f>
+        <v>233</v>
+      </c>
+      <c r="F7" s="8">
+        <v>515</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1176</v>
+      </c>
+      <c r="H7" s="8">
+        <v>181</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" si="0"/>
+        <v>4055</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>48660</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>45.387599999999999</v>
+      </c>
+      <c r="C8">
+        <v>-75.695999999999998</v>
+      </c>
+      <c r="D8">
+        <v>1859</v>
+      </c>
+      <c r="E8" s="8">
+        <f>84+168</f>
+        <v>252</v>
+      </c>
+      <c r="F8" s="8">
+        <v>578</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1194</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1018</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="0"/>
+        <v>4901</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>58812</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>45.504800000000003</v>
+      </c>
+      <c r="C9">
+        <v>-73.613200000000006</v>
+      </c>
+      <c r="D9">
+        <v>1425</v>
+      </c>
+      <c r="E9" s="8">
+        <f>73+160</f>
+        <v>233</v>
+      </c>
+      <c r="F9" s="8">
+        <v>515</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1176</v>
+      </c>
+      <c r="H9" s="8">
+        <v>181</v>
+      </c>
+      <c r="I9" s="7">
+        <f t="shared" si="0"/>
+        <v>3530</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>42360</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10">
+        <v>52.133400000000002</v>
+      </c>
+      <c r="C10">
+        <v>-106.6314</v>
+      </c>
+      <c r="D10">
+        <v>1137</v>
+      </c>
+      <c r="E10" s="8">
+        <f>168+201</f>
+        <v>369</v>
+      </c>
+      <c r="F10" s="8">
+        <v>530</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1194</v>
+      </c>
+      <c r="H10" s="8">
+        <v>750</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="0"/>
+        <v>3980</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>47760</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11">
+        <v>47.573799999999999</v>
+      </c>
+      <c r="C11">
+        <v>-52.732900000000001</v>
+      </c>
+      <c r="D11">
+        <v>908</v>
+      </c>
+      <c r="E11" s="8">
+        <f>130+174</f>
+        <v>304</v>
+      </c>
+      <c r="F11" s="8">
+        <v>578</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1080</v>
+      </c>
+      <c r="H11" s="8">
+        <v>651</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="0"/>
+        <v>3521</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>42252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>43.657699999999998</v>
+      </c>
+      <c r="C12">
+        <v>-79.378799999999998</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2499</v>
+      </c>
+      <c r="E12" s="7">
+        <f>104+168</f>
+        <v>272</v>
+      </c>
+      <c r="F12" s="8">
+        <v>578</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1194</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1250</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="0"/>
+        <v>5793</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>69516</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>49.260599999999997</v>
+      </c>
+      <c r="C13">
+        <v>-123.246</v>
+      </c>
+      <c r="D13">
+        <v>3500</v>
+      </c>
+      <c r="E13" s="8">
+        <f>116+174</f>
+        <v>290</v>
+      </c>
+      <c r="F13" s="8">
+        <v>649</v>
+      </c>
+      <c r="G13" s="8">
+        <v>1218</v>
+      </c>
+      <c r="H13" s="8">
+        <v>935</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="0"/>
+        <v>6592</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>79104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14">
+        <v>49.807499999999997</v>
+      </c>
+      <c r="C14">
+        <v>-97.136600000000001</v>
+      </c>
+      <c r="D14">
+        <v>1375</v>
+      </c>
+      <c r="E14" s="8">
+        <f>94+174</f>
+        <v>268</v>
+      </c>
+      <c r="F14" s="8">
+        <v>523</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1140</v>
+      </c>
+      <c r="H14" s="8">
+        <v>451</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="0"/>
+        <v>3757</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15">
+        <v>46.256900000000002</v>
+      </c>
+      <c r="C15">
+        <v>-63.1389</v>
+      </c>
+      <c r="D15">
+        <v>1290</v>
+      </c>
+      <c r="E15" s="7">
+        <f>174+177</f>
+        <v>351</v>
+      </c>
+      <c r="F15" s="7">
+        <f>AVERAGE(F2:F14)</f>
+        <v>548</v>
+      </c>
+      <c r="G15" s="7">
+        <f>308*3</f>
+        <v>924</v>
+      </c>
+      <c r="H15" s="8">
+        <v>568</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" si="0"/>
+        <v>3681</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>44172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="25" spans="4:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G30" s="4"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:K26">
+    <sortCondition ref="A21:A26"/>
+  </sortState>
+  <conditionalFormatting sqref="A7:C7 A15:C44 A8:A14 A1:A6">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E8" formula="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F162D4F-4FC6-474B-BB43-16544EB64190}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,36 +2873,36 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1561,18 +2910,29 @@
     </row>
     <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>